<commit_message>
Align WHO Hepatitis A and Rubella with current WHO guidance
- HepA: convert from universal Standard to Risk series, add single-dose
  series (WHO 2022 for intermediate/high endemicity) as primary option,
  keep 2-dose as alternative, add observation code 1027, remove
  latestRecAge cap from dose 2
- Rubella: split into two series for different country schedules —
  9-month first dose (ongoing transmission, dose 2 at 15mo) and
  12-month first dose (low transmission, dose 2 at 4y). Fix dose 2
  absMinAge based on interval (10mo/13mo), remove latestRecAge caps

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/HepA.xlsx
+++ b/cicada_generator/lib/WHO/antigen/HepA.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="2-dose series" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="1-dose series" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="2-dose series" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,96 +13,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="36">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
+    <t xml:space="preserve">WHO HepA single-dose series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target Disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HepA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccine Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Series Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equivalent Series Groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Patient Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lives in HepA intermediate/high endemicity area (1027)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient lives in a hepatitis A intermediate or high endemicity area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Series Dose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dose 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferable Vaccine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HepA, pediatric/adolescent (83)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowable Vaccine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HepA, adult (52)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HepA-HepB (Twinrix) (104)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurring Dose</t>
+  </si>
+  <si>
     <t xml:space="preserve">WHO HepA 2-dose series</t>
   </si>
   <si>
-    <t xml:space="preserve">Target Disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HepA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccine Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Series Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equivalent Series Groups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select Patient Series</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Series Dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferable Vaccine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HepA, pediatric/adolescent (83)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allowable Vaccine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HepA, adult (52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HepA-HepB (Twinrix) (104)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurring Dose</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">Dose 2</t>
   </si>
   <si>
     <t xml:space="preserve">18 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 months</t>
   </si>
   <si>
     <t xml:space="preserve">Preferable Interval</t>
@@ -416,10 +429,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -444,54 +457,42 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -499,24 +500,33 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -524,13 +534,13 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -538,93 +548,262 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -633,10 +812,16 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -644,24 +829,33 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -669,13 +863,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -683,10 +877,24 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>